<commit_message>
added centre overview data
</commit_message>
<xml_diff>
--- a/Student Improvement Status.xlsx
+++ b/Student Improvement Status.xlsx
@@ -559,38 +559,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -6771,17 +6740,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:N130">
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
-      <formula>"gain"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
-      <formula>"loss"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
-      <formula>"no change"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="G2:G130">
     <cfRule type="colorScale" priority="3">
       <colorScale>

</xml_diff>

<commit_message>
added charts for all aes data
</commit_message>
<xml_diff>
--- a/Student Improvement Status.xlsx
+++ b/Student Improvement Status.xlsx
@@ -1123,13 +1123,13 @@
         <v>95</v>
       </c>
       <c r="D2">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E2">
         <v>83</v>
       </c>
       <c r="F2">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1143,7 +1143,7 @@
         <v>17</v>
       </c>
       <c r="D3">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E3">
         <v>24</v>
@@ -1163,13 +1163,13 @@
         <v>17</v>
       </c>
       <c r="D4">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E4">
         <v>22</v>
       </c>
       <c r="F4">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1308,7 +1308,7 @@
         <v>5.5</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="K3">
         <v>6</v>
@@ -1440,7 +1440,7 @@
         <v>5</v>
       </c>
       <c r="J6">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="K6">
         <v>6</v>
@@ -1452,7 +1452,7 @@
         <v>6</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -1572,7 +1572,7 @@
         <v>5</v>
       </c>
       <c r="J9">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="K9">
         <v>5.5</v>
@@ -1616,7 +1616,7 @@
         <v>5.5</v>
       </c>
       <c r="J10">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="K10">
         <v>6.5</v>
@@ -1672,7 +1672,7 @@
         <v>5</v>
       </c>
       <c r="N11">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -1792,7 +1792,7 @@
         <v>5</v>
       </c>
       <c r="J14">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="K14">
         <v>6</v>
@@ -2012,7 +2012,7 @@
         <v>5.5</v>
       </c>
       <c r="J19">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="K19">
         <v>7</v>
@@ -2144,7 +2144,7 @@
         <v>5</v>
       </c>
       <c r="J22">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="K22">
         <v>6</v>
@@ -2188,7 +2188,7 @@
         <v>5</v>
       </c>
       <c r="J23">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="K23">
         <v>5.5</v>
@@ -2320,7 +2320,7 @@
         <v>6</v>
       </c>
       <c r="J26">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="K26">
         <v>7</v>
@@ -2804,7 +2804,7 @@
         <v>6</v>
       </c>
       <c r="J37">
-        <v>-1</v>
+        <v>-1.5</v>
       </c>
       <c r="K37">
         <v>6</v>
@@ -3068,7 +3068,7 @@
         <v>5.5</v>
       </c>
       <c r="J43">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="K43">
         <v>6</v>
@@ -3200,7 +3200,7 @@
         <v>5</v>
       </c>
       <c r="J46">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="K46">
         <v>5</v>
@@ -3288,7 +3288,7 @@
         <v>5.5</v>
       </c>
       <c r="J48">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="K48">
         <v>4.5</v>
@@ -3464,7 +3464,7 @@
         <v>5.5</v>
       </c>
       <c r="J52">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="K52">
         <v>6</v>
@@ -3640,7 +3640,7 @@
         <v>6</v>
       </c>
       <c r="J56">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="K56">
         <v>6</v>
@@ -4036,7 +4036,7 @@
         <v>5</v>
       </c>
       <c r="J65">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="K65">
         <v>5.5</v>
@@ -4124,7 +4124,7 @@
         <v>6</v>
       </c>
       <c r="J67">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="K67">
         <v>6</v>
@@ -4168,7 +4168,7 @@
         <v>6</v>
       </c>
       <c r="J68">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="K68">
         <v>6.5</v>
@@ -4212,7 +4212,7 @@
         <v>6.5</v>
       </c>
       <c r="J69">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="K69">
         <v>7.5</v>
@@ -4300,7 +4300,7 @@
         <v>5</v>
       </c>
       <c r="J71">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="K71">
         <v>6</v>
@@ -4388,7 +4388,7 @@
         <v>6</v>
       </c>
       <c r="J73">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="K73">
         <v>7.5</v>
@@ -4564,7 +4564,7 @@
         <v>6.5</v>
       </c>
       <c r="J77">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="K77">
         <v>9</v>
@@ -4696,7 +4696,7 @@
         <v>6.5</v>
       </c>
       <c r="J80">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="K80">
         <v>6.5</v>
@@ -4740,7 +4740,7 @@
         <v>5</v>
       </c>
       <c r="J81">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="K81">
         <v>8</v>
@@ -4784,7 +4784,7 @@
         <v>6</v>
       </c>
       <c r="J82">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="K82">
         <v>7</v>
@@ -4916,7 +4916,7 @@
         <v>6</v>
       </c>
       <c r="J85">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="K85">
         <v>7</v>
@@ -5356,7 +5356,7 @@
         <v>6</v>
       </c>
       <c r="J95">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="K95">
         <v>7</v>
@@ -5412,7 +5412,7 @@
         <v>5.5</v>
       </c>
       <c r="N96">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="97" spans="1:14">
@@ -5444,7 +5444,7 @@
         <v>5.5</v>
       </c>
       <c r="J97">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K97">
         <v>5.5</v>
@@ -5456,7 +5456,7 @@
         <v>5.5</v>
       </c>
       <c r="N97">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:14">
@@ -5620,7 +5620,7 @@
         <v>6</v>
       </c>
       <c r="J101">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="K101">
         <v>7</v>
@@ -5796,7 +5796,7 @@
         <v>6</v>
       </c>
       <c r="J105">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K105">
         <v>7.5</v>
@@ -6380,7 +6380,7 @@
         <v>5.5</v>
       </c>
       <c r="N118">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:14">
@@ -6896,7 +6896,7 @@
         <v>8</v>
       </c>
       <c r="J130">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="K130">
         <v>8.5</v>
@@ -6908,7 +6908,7 @@
         <v>8</v>
       </c>
       <c r="N130">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>